<commit_message>
začátek dodávání souřadnic do gisu
</commit_message>
<xml_diff>
--- a/longitude - latitude/newtonuv_mozek-toponyma.xlsx
+++ b/longitude - latitude/newtonuv_mozek-toponyma.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\korpus_prozy\korpusprozy\longitude - latitude\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E6C6EB-8B90-4E6D-9618-7C7B7585B52F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6881D20-3CBE-45C7-97D5-B2C935D407E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="168" windowWidth="6744" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1481,8 +1481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D119" sqref="D119"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
pokrok v newtonově mozku
</commit_message>
<xml_diff>
--- a/longitude - latitude/newtonuv_mozek-toponyma.xlsx
+++ b/longitude - latitude/newtonuv_mozek-toponyma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\korpus_prozy\korpusprozy\longitude - latitude\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6881D20-3CBE-45C7-97D5-B2C935D407E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C8805D0-EA80-4335-8BDE-56F1686AA507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="168" windowWidth="6744" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="360">
   <si>
     <t>longitude</t>
   </si>
@@ -1097,6 +1097,9 @@
   </si>
   <si>
     <t>9.1750717</t>
+  </si>
+  <si>
+    <t>musím najít vhodný obrázek</t>
   </si>
 </sst>
 </file>
@@ -1481,8 +1484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D124"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1649,6 +1652,9 @@
       <c r="C14" t="s">
         <v>106</v>
       </c>
+      <c r="D14" t="s">
+        <v>359</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">

</xml_diff>